<commit_message>
deleted extraneous files & outdated versions of datasets
</commit_message>
<xml_diff>
--- a/widthHCcombined.xlsx
+++ b/widthHCcombined.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="0" windowWidth="13120" windowHeight="16540" tabRatio="659" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="659"/>
   </bookViews>
   <sheets>
     <sheet name="ColdYounger" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="115">
   <si>
     <t>Ind48_right_60xobj_YAYHAIR</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>Indiv6L_c262_40x_second(typo-c292)</t>
-  </si>
-  <si>
-    <t>flat position so didn't measure many</t>
   </si>
   <si>
     <t>Indiv147L_c428_60x_second</t>
@@ -949,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E345"/>
   <sheetViews>
-    <sheetView topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="A333" sqref="A333"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1781,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <f t="shared" ref="E66:E97" si="2">C66*D66</f>
+        <f t="shared" ref="E66:E67" si="2">C66*D66</f>
         <v>6</v>
       </c>
     </row>
@@ -5247,8 +5244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E475"/>
   <sheetViews>
-    <sheetView topLeftCell="A447" workbookViewId="0">
-      <selection activeCell="A443" sqref="A443"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11107,10 +11104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F297"/>
+  <dimension ref="A1:E297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="D226" sqref="D226"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13298,7 +13295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:5">
       <c r="C177" s="2">
         <v>3</v>
       </c>
@@ -13310,7 +13307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:5">
       <c r="C178" s="2">
         <v>2</v>
       </c>
@@ -13322,7 +13319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:5">
       <c r="C179" s="2">
         <v>2</v>
       </c>
@@ -13334,7 +13331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:5">
       <c r="C180" s="2">
         <v>2</v>
       </c>
@@ -13346,7 +13343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:5">
       <c r="C181" s="2">
         <v>2</v>
       </c>
@@ -13358,7 +13355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:5">
       <c r="C182" s="2">
         <v>3</v>
       </c>
@@ -13370,7 +13367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:5">
       <c r="C183" s="2">
         <v>2</v>
       </c>
@@ -13382,7 +13379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:5">
       <c r="C184" s="2">
         <v>2</v>
       </c>
@@ -13394,7 +13391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:5">
       <c r="C185" s="2">
         <v>3</v>
       </c>
@@ -13406,7 +13403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:5">
       <c r="C186" s="2">
         <v>2</v>
       </c>
@@ -13418,7 +13415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:5">
       <c r="C187" s="2">
         <v>2</v>
       </c>
@@ -13430,7 +13427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:5">
       <c r="C188" s="2">
         <v>2</v>
       </c>
@@ -13442,7 +13439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:5">
       <c r="C189" s="2">
         <v>3</v>
       </c>
@@ -13454,7 +13451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
         <v>65</v>
       </c>
@@ -13471,11 +13468,8 @@
         <f>C190*D190</f>
         <v>8</v>
       </c>
-      <c r="F190" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6">
+    </row>
+    <row r="191" spans="1:5">
       <c r="C191" s="2">
         <v>4</v>
       </c>
@@ -13487,7 +13481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:5">
       <c r="C192" s="2">
         <v>3</v>
       </c>
@@ -13501,7 +13495,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B193" t="s">
         <v>45</v>
@@ -13723,7 +13717,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B211" t="s">
         <v>45</v>
@@ -13849,7 +13843,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B221" t="s">
         <v>45</v>
@@ -13939,7 +13933,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B228" t="s">
         <v>41</v>
@@ -14695,7 +14689,7 @@
   <dimension ref="A1:E410"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C405" sqref="C399:E405"/>
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19759,8 +19753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E400"/>
   <sheetViews>
-    <sheetView topLeftCell="A378" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24680,8 +24674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E410"/>
   <sheetViews>
-    <sheetView topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211:XFD410"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -29530,12 +29524,14 @@
   <dimension ref="A1:E430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="4"/>
+    <col min="1" max="1" width="14.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="10.6640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>